<commit_message>
Modified the task list
</commit_message>
<xml_diff>
--- a/ECE 4981 Task List.xlsx
+++ b/ECE 4981 Task List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fall2020\4981 Senior Design 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fall2020\ECE4981\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EC4B35-CFD8-48E3-83EC-6F371120F514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538710C9-DC76-4653-974C-C808059CB7BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B8829020-0EF2-4875-8210-9C2942B344E7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>START DATE</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Draft Concept Description with advisor comments</t>
   </si>
   <si>
-    <t>When meeting on Sep 8, we should discuss and determine the sub-tasks for this task.</t>
-  </si>
-  <si>
     <t>Present Concept Description</t>
   </si>
   <si>
@@ -188,6 +185,26 @@
   <si>
     <t>The task list used to keep track of the main tasks and sub-tasks that need to be done in order to complete the senior design project. The task list also includes dates, priorities, assignees' initials, status, and comments.
 09/05/20 Created the template for the task list. Will add more tasks, sub-tasks and deadline later.</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>When meeting on Sep 8, we should discuss and determine the sub-tasks for this task.
+Wait until receiving template from prof</t>
+  </si>
+  <si>
+    <t>3 team members</t>
+  </si>
+  <si>
+    <t>Sound Logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/08/20 
+How many advisors can we have?
+Prof Putty (backup Prof: John Miller, Larry Sieh, Azeem H.)
+Contact and Set up a meeting with the advisor
+</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1159,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -1207,7 +1224,7 @@
       <c r="I2" s="35"/>
       <c r="J2" s="2"/>
       <c r="L2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>16</v>
@@ -1287,13 +1304,13 @@
       </c>
       <c r="G5" s="10">
         <f ca="1">(NETWORKDAYS.INTL(TODAY(),F5))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1329,7 +1346,7 @@
       </c>
       <c r="G7" s="10">
         <f ca="1">(NETWORKDAYS.INTL(TODAY(),F7))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>18</v>
@@ -1350,8 +1367,12 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="J8" s="2"/>
       <c r="L8" s="2"/>
     </row>
@@ -1365,8 +1386,12 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="J9" s="2"/>
       <c r="L9" s="2"/>
     </row>
@@ -1395,23 +1420,31 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="101.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="10"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -1429,7 +1462,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
         <v>3</v>
       </c>
@@ -1448,13 +1481,13 @@
       </c>
       <c r="G14" s="10">
         <f t="shared" ref="G14" ca="1" si="0">(NETWORKDAYS.INTL(TODAY(),F14))</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1535,7 +1568,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>15</v>
@@ -1549,10 +1582,10 @@
       </c>
       <c r="G20" s="10">
         <f t="shared" ref="G20" ca="1" si="1">(NETWORKDAYS.INTL(TODAY(),F20))</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="2"/>
@@ -1620,7 +1653,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>16</v>
@@ -1634,10 +1667,10 @@
       </c>
       <c r="G25" s="10">
         <f t="shared" ref="G25" ca="1" si="2">(NETWORKDAYS.INTL(TODAY(),F25))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="2"/>
@@ -1727,7 +1760,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>16</v>
@@ -1741,10 +1774,10 @@
       </c>
       <c r="G32" s="10">
         <f t="shared" ref="G32" ca="1" si="3">(NETWORKDAYS.INTL(TODAY(),F32))</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I32" s="18"/>
     </row>
@@ -1819,7 +1852,7 @@
         <v>7</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>16</v>
@@ -1833,7 +1866,7 @@
       </c>
       <c r="G39" s="10">
         <f t="shared" ref="G39" ca="1" si="4">(NETWORKDAYS.INTL(TODAY(),F39))</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H39" s="21"/>
       <c r="I39" s="18"/>
@@ -1909,7 +1942,7 @@
         <v>8</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>16</v>
@@ -1923,10 +1956,10 @@
       </c>
       <c r="G46" s="10">
         <f t="shared" ref="G46" ca="1" si="5">(NETWORKDAYS.INTL(TODAY(),F46))</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I46" s="18"/>
     </row>
@@ -1990,7 +2023,7 @@
         <v>9</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C52" s="21" t="s">
         <v>16</v>
@@ -2004,10 +2037,10 @@
       </c>
       <c r="G52" s="10">
         <f t="shared" ref="G52" ca="1" si="6">(NETWORKDAYS.INTL(TODAY(),F52))</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H52" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I52" s="18"/>
     </row>
@@ -2071,7 +2104,7 @@
         <v>10</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C58" s="21" t="s">
         <v>16</v>
@@ -2085,10 +2118,10 @@
       </c>
       <c r="G58" s="10">
         <f t="shared" ref="G58" ca="1" si="7">(NETWORKDAYS.INTL(TODAY(),F58))</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H58" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I58" s="18"/>
     </row>
@@ -2152,7 +2185,7 @@
         <v>11</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C64" s="21" t="s">
         <v>16</v>
@@ -2166,10 +2199,10 @@
       </c>
       <c r="G64" s="10">
         <f t="shared" ref="G64" ca="1" si="8">(NETWORKDAYS.INTL(TODAY(),F64))</f>
+        <v>35</v>
+      </c>
+      <c r="H64" s="21" t="s">
         <v>36</v>
-      </c>
-      <c r="H64" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="I64" s="18"/>
     </row>
@@ -2233,7 +2266,7 @@
         <v>12</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C70" s="21" t="s">
         <v>16</v>
@@ -2247,10 +2280,10 @@
       </c>
       <c r="G70" s="10">
         <f t="shared" ref="G70" ca="1" si="9">(NETWORKDAYS.INTL(TODAY(),F70))</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H70" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I70" s="18"/>
     </row>
@@ -2314,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C76" s="21" t="s">
         <v>16</v>
@@ -2328,7 +2361,7 @@
       </c>
       <c r="G76" s="10">
         <f t="shared" ref="G76" ca="1" si="10">(NETWORKDAYS.INTL(TODAY(),F76))</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H76" s="21"/>
       <c r="I76" s="18"/>
@@ -2393,7 +2426,7 @@
         <v>14</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C82" s="21" t="s">
         <v>16</v>
@@ -2467,7 +2500,7 @@
         <v>15</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C88" s="21" t="s">
         <v>16</v>
@@ -2481,7 +2514,7 @@
       </c>
       <c r="G88" s="10">
         <f t="shared" ref="G88" ca="1" si="11">(NETWORKDAYS.INTL(TODAY(),F88))</f>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H88" s="21"/>
       <c r="I88" s="18"/>
@@ -2546,7 +2579,7 @@
         <v>16</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C94" s="21" t="s">
         <v>16</v>
@@ -2620,7 +2653,7 @@
         <v>17</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C100" s="21" t="s">
         <v>16</v>
@@ -2634,7 +2667,7 @@
       </c>
       <c r="G100" s="10">
         <f t="shared" ref="G100" ca="1" si="12">(NETWORKDAYS.INTL(TODAY(),F100))</f>
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H100" s="21"/>
       <c r="I100" s="18"/>
@@ -2710,7 +2743,7 @@
         <v>18</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C107" s="21" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Adding subtasks for Task 3
</commit_message>
<xml_diff>
--- a/ECE 4981 Task List.xlsx
+++ b/ECE 4981 Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fall2020\ECE4981\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBAAD5B-2940-4228-BA49-B0E040502F67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCAE7F6-88B6-4909-ADC2-55B6C374B8BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B8829020-0EF2-4875-8210-9C2942B344E7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
   <si>
     <t>START DATE</t>
   </si>
@@ -194,10 +194,6 @@
     <t>Sound Logic</t>
   </si>
   <si>
-    <t xml:space="preserve">09/08/20 Matt to document the problems
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">09/10/2020 Professor Paul Watta has accepted our invitation to be our faculty advisor. Matt Falconer will set up a vrtual meeting with him for next week in which we can discuss our project concepts and receive written advisor comments.
 </t>
   </si>
@@ -212,6 +208,19 @@
   </si>
   <si>
     <t>09/11/20 HD to make a ppt slides to present what should be included in a concept description before next group meeting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/08/20 Matt to the working principle of a resonator
+</t>
+  </si>
+  <si>
+    <t>Team meeting to assign tasks on draft concept description</t>
+  </si>
+  <si>
+    <t>Send a draft concept description to Prof Watta and set up a meeting with Prof</t>
+  </si>
+  <si>
+    <t>Meet with Prof Watta to have inputs, thoughts, comments</t>
   </si>
 </sst>
 </file>
@@ -1164,9 +1173,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ADCF63-C9C4-4C77-9C8F-0AE89C3F3266}">
   <dimension ref="A1:O995"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -1200,7 +1209,7 @@
       <c r="F1" s="33"/>
       <c r="G1" s="33"/>
       <c r="H1" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I1" s="34"/>
       <c r="J1" s="2"/>
@@ -1226,7 +1235,7 @@
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
       <c r="H2" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="35"/>
       <c r="J2" s="2"/>
@@ -1340,7 +1349,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>27</v>
@@ -1422,8 +1431,12 @@
       <c r="B11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="10"/>
@@ -1431,7 +1444,7 @@
         <v>18</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="J11" s="2"/>
       <c r="L11" s="2"/>
@@ -1451,10 +1464,10 @@
       <c r="F12" s="9"/>
       <c r="G12" s="10"/>
       <c r="H12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1481,7 +1494,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>27</v>
@@ -1495,7 +1508,7 @@
         <v>6</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>48</v>
@@ -1507,11 +1520,9 @@
     <row r="15" spans="1:15" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>20</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
         <v>13</v>
       </c>
@@ -1529,17 +1540,21 @@
         <v>18</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="14"/>
+      <c r="B16" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="10"/>
@@ -1549,9 +1564,11 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
+      <c r="B17" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="9"/>
@@ -1563,9 +1580,11 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="14"/>
+      <c r="B18" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="9"/>

</xml_diff>

<commit_message>
modified Admin task list
</commit_message>
<xml_diff>
--- a/ECE 4981 Task List.xlsx
+++ b/ECE 4981 Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fall2020\ECE4981\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479D8969-7FB9-4FAF-AC82-45346CF16E34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E769176D-548A-463D-AC19-3C21E369A7F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8829020-0EF2-4875-8210-9C2942B344E7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="97">
   <si>
     <t>START DATE</t>
   </si>
@@ -323,6 +323,21 @@
 09/12/20 Have gathered info from all posible good sources for the documentation. Sources: Prof Paul Richarson, ECE4951, and Embedded Systems - Shape the World Micocontroller I/O by Valvano.
 09/14/20 The team will use the concept description template provided by the Professor. Instead, sharing Development Process by ECE4951 and Valvano Embedded Sys
 </t>
+  </si>
+  <si>
+    <t>Functional Char of the projects. What it does with the diagram</t>
+  </si>
+  <si>
+    <t>Risk management</t>
+  </si>
+  <si>
+    <t>ROM &amp; Modules status</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Determine problems (cost, performance, automation)</t>
   </si>
 </sst>
 </file>
@@ -634,6 +649,9 @@
     <xf numFmtId="1" fontId="1" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -641,9 +659,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1682,11 +1697,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ADCF63-C9C4-4C77-9C8F-0AE89C3F3266}">
-  <dimension ref="A1:P995"/>
+  <dimension ref="A1:P998"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
@@ -1711,20 +1726,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
       <c r="L1" s="2" t="s">
         <v>10</v>
@@ -1740,18 +1755,18 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="45" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
       <c r="M2" s="3" t="s">
         <v>32</v>
@@ -1761,18 +1776,18 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="45" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
       <c r="M3" s="3" t="s">
         <v>16</v>
@@ -2067,7 +2082,7 @@
       <c r="H15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="46" t="s">
+      <c r="I15" s="43" t="s">
         <v>90</v>
       </c>
       <c r="J15" s="34" t="s">
@@ -2077,64 +2092,60 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="42" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="6"/>
+    <row r="16" spans="1:16" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="D16" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8">
-        <v>44091</v>
-      </c>
-      <c r="G16" s="9">
-        <f ca="1">IF(H16="Done",0,(NETWORKDAYS.INTL(TODAY(),F16)))</f>
-        <v>3</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="34"/>
+        <v>44089</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="34" t="s">
+        <v>96</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="C17" s="14"/>
-      <c r="D17" s="14" t="s">
-        <v>45</v>
+      <c r="D17" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8">
         <v>44090</v>
       </c>
-      <c r="G17" s="9">
-        <f ca="1">IF(H17="Done",0,(NETWORKDAYS.INTL(TODAY(),F17)))</f>
-        <v>2</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="34"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="34" t="s">
+        <v>95</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="6"/>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="14"/>
       <c r="D18" s="6" t="s">
         <v>25</v>
       </c>
@@ -2142,54 +2153,58 @@
       <c r="F18" s="8">
         <v>44091</v>
       </c>
-      <c r="G18" s="9">
-        <f ca="1">IF(H18="Done",0,(NETWORKDAYS.INTL(TODAY(),F18)))</f>
-        <v>3</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="34"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="34" t="s">
+        <v>95</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+    <row r="19" spans="1:13" ht="42" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="3"/>
+      <c r="F19" s="8">
+        <v>44091</v>
+      </c>
+      <c r="G19" s="9">
+        <f ca="1">IF(H19="Done",0,(NETWORKDAYS.INTL(TODAY(),F19)))</f>
+        <v>3</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="I19" s="3"/>
       <c r="J19" s="34"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="26">
-        <v>4</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>25</v>
+    <row r="20" spans="1:13" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8">
-        <v>44095</v>
+        <v>44090</v>
       </c>
       <c r="G20" s="9">
         <f ca="1">IF(H20="Done",0,(NETWORKDAYS.INTL(TODAY(),F20)))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>32</v>
@@ -2200,90 +2215,101 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+    <row r="21" spans="1:13" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="3"/>
+      <c r="F21" s="8">
+        <v>44091</v>
+      </c>
+      <c r="G21" s="9">
+        <f ca="1">IF(H21="Done",0,(NETWORKDAYS.INTL(TODAY(),F21)))</f>
+        <v>3</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="I21" s="3"/>
       <c r="J21" s="34"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="35"/>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="34"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="35"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="26">
+        <v>4</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8">
+        <v>44095</v>
+      </c>
+      <c r="G23" s="9">
+        <f ca="1">IF(H23="Done",0,(NETWORKDAYS.INTL(TODAY(),F23)))</f>
+        <v>5</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="34"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="35"/>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="34"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="28">
-        <v>5</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A25" s="20"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="21">
-        <v>44099</v>
-      </c>
-      <c r="G25" s="9">
-        <f ca="1">IF(H25="Done",0,(NETWORKDAYS.INTL(TODAY(),F25)))</f>
-        <v>9</v>
-      </c>
-      <c r="H25" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="20"/>
       <c r="J25" s="35"/>
       <c r="K25" s="1"/>
@@ -2321,14 +2347,29 @@
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
+      <c r="A28" s="28">
+        <v>5</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="F28" s="21">
+        <v>44099</v>
+      </c>
+      <c r="G28" s="9">
+        <f ca="1">IF(H28="Done",0,(NETWORKDAYS.INTL(TODAY(),F28)))</f>
+        <v>9</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="I28" s="20"/>
       <c r="J28" s="35"/>
       <c r="K28" s="1"/>
@@ -2361,6 +2402,9 @@
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="35"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="20"/>
@@ -2373,33 +2417,24 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
       <c r="J31" s="35"/>
-    </row>
-    <row r="32" spans="1:13" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="28">
-        <v>6</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="20"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="21"/>
-      <c r="F32" s="21">
-        <v>44106</v>
-      </c>
-      <c r="G32" s="9">
-        <f ca="1">IF(H32="Done",0,(NETWORKDAYS.INTL(TODAY(),F32)))</f>
-        <v>14</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="F32" s="21"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="35"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
@@ -2425,15 +2460,30 @@
       <c r="I34" s="20"/>
       <c r="J34" s="35"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+    <row r="35" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="28">
+        <v>6</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
+      <c r="F35" s="21">
+        <v>44106</v>
+      </c>
+      <c r="G35" s="9">
+        <f ca="1">IF(H35="Done",0,(NETWORKDAYS.INTL(TODAY(),F35)))</f>
+        <v>14</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="I35" s="20"/>
       <c r="J35" s="35"/>
     </row>
@@ -2474,26 +2524,13 @@
       <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="28">
-        <v>7</v>
-      </c>
-      <c r="B39" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A39" s="20"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="21"/>
-      <c r="F39" s="21">
-        <v>44113</v>
-      </c>
-      <c r="G39" s="9">
-        <f ca="1">IF(H39="Done",0,(NETWORKDAYS.INTL(TODAY(),F39)))</f>
-        <v>19</v>
-      </c>
+      <c r="F39" s="21"/>
+      <c r="G39" s="20"/>
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
       <c r="J39" s="35"/>
@@ -2523,13 +2560,26 @@
       <c r="J41" s="35"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="20"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
+      <c r="A42" s="28">
+        <v>7</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="20"/>
+      <c r="F42" s="21">
+        <v>44113</v>
+      </c>
+      <c r="G42" s="9">
+        <f ca="1">IF(H42="Done",0,(NETWORKDAYS.INTL(TODAY(),F42)))</f>
+        <v>19</v>
+      </c>
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
       <c r="J42" s="35"/>
@@ -2571,29 +2621,14 @@
       <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="28">
-        <v>8</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A46" s="20"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="21"/>
-      <c r="F46" s="21">
-        <v>44120</v>
-      </c>
-      <c r="G46" s="9">
-        <f ca="1">IF(H46="Done",0,(NETWORKDAYS.INTL(TODAY(),F46)))</f>
-        <v>24</v>
-      </c>
-      <c r="H46" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="F46" s="21"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
       <c r="I46" s="20"/>
       <c r="J46" s="35"/>
     </row>
@@ -2622,14 +2657,29 @@
       <c r="J48" s="35"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
+      <c r="A49" s="28">
+        <v>8</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
+      <c r="F49" s="21">
+        <v>44120</v>
+      </c>
+      <c r="G49" s="9">
+        <f ca="1">IF(H49="Done",0,(NETWORKDAYS.INTL(TODAY(),F49)))</f>
+        <v>24</v>
+      </c>
+      <c r="H49" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="I49" s="20"/>
       <c r="J49" s="35"/>
     </row>
@@ -2658,29 +2708,14 @@
       <c r="J51" s="35"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="28">
-        <v>9</v>
-      </c>
-      <c r="B52" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A52" s="20"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
       <c r="E52" s="21"/>
-      <c r="F52" s="21">
-        <v>44123</v>
-      </c>
-      <c r="G52" s="9">
-        <f ca="1">IF(H52="Done",0,(NETWORKDAYS.INTL(TODAY(),F52)))</f>
-        <v>25</v>
-      </c>
-      <c r="H52" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="F52" s="21"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
       <c r="I52" s="20"/>
       <c r="J52" s="35"/>
     </row>
@@ -2709,14 +2744,29 @@
       <c r="J54" s="35"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="20"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
+      <c r="A55" s="28">
+        <v>9</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
+      <c r="F55" s="21">
+        <v>44123</v>
+      </c>
+      <c r="G55" s="9">
+        <f ca="1">IF(H55="Done",0,(NETWORKDAYS.INTL(TODAY(),F55)))</f>
+        <v>25</v>
+      </c>
+      <c r="H55" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="I55" s="20"/>
       <c r="J55" s="35"/>
     </row>
@@ -2744,30 +2794,15 @@
       <c r="I57" s="20"/>
       <c r="J57" s="35"/>
     </row>
-    <row r="58" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A58" s="28">
-        <v>10</v>
-      </c>
-      <c r="B58" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>25</v>
-      </c>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="20"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
       <c r="E58" s="21"/>
-      <c r="F58" s="21">
-        <v>44127</v>
-      </c>
-      <c r="G58" s="9">
-        <f ca="1">IF(H58="Done",0,(NETWORKDAYS.INTL(TODAY(),F58)))</f>
-        <v>29</v>
-      </c>
-      <c r="H58" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="F58" s="21"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
       <c r="I58" s="20"/>
       <c r="J58" s="35"/>
     </row>
@@ -2795,15 +2830,30 @@
       <c r="I60" s="20"/>
       <c r="J60" s="35"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="20"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
+    <row r="61" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A61" s="28">
+        <v>10</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
+      <c r="F61" s="21">
+        <v>44127</v>
+      </c>
+      <c r="G61" s="9">
+        <f ca="1">IF(H61="Done",0,(NETWORKDAYS.INTL(TODAY(),F61)))</f>
+        <v>29</v>
+      </c>
+      <c r="H61" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="I61" s="20"/>
       <c r="J61" s="35"/>
     </row>
@@ -2832,29 +2882,14 @@
       <c r="J63" s="35"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="28">
-        <v>11</v>
-      </c>
-      <c r="B64" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A64" s="20"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
       <c r="E64" s="21"/>
-      <c r="F64" s="21">
-        <v>44130</v>
-      </c>
-      <c r="G64" s="9">
-        <f ca="1">IF(H64="Done",0,(NETWORKDAYS.INTL(TODAY(),F64)))</f>
-        <v>30</v>
-      </c>
-      <c r="H64" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="F64" s="21"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
       <c r="I64" s="20"/>
       <c r="J64" s="35"/>
     </row>
@@ -2883,14 +2918,29 @@
       <c r="J66" s="35"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="20"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
+      <c r="A67" s="28">
+        <v>11</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="20"/>
-      <c r="H67" s="20"/>
+      <c r="F67" s="21">
+        <v>44130</v>
+      </c>
+      <c r="G67" s="9">
+        <f ca="1">IF(H67="Done",0,(NETWORKDAYS.INTL(TODAY(),F67)))</f>
+        <v>30</v>
+      </c>
+      <c r="H67" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="I67" s="20"/>
       <c r="J67" s="35"/>
     </row>
@@ -2918,30 +2968,15 @@
       <c r="I69" s="20"/>
       <c r="J69" s="35"/>
     </row>
-    <row r="70" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="28">
-        <v>12</v>
-      </c>
-      <c r="B70" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C70" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>25</v>
-      </c>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="20"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
       <c r="E70" s="21"/>
-      <c r="F70" s="21">
-        <v>44141</v>
-      </c>
-      <c r="G70" s="9">
-        <f ca="1">IF(H70="Done",0,(NETWORKDAYS.INTL(TODAY(),F70)))</f>
-        <v>39</v>
-      </c>
-      <c r="H70" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="F70" s="21"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20"/>
       <c r="I70" s="20"/>
       <c r="J70" s="35"/>
     </row>
@@ -2969,15 +3004,30 @@
       <c r="I72" s="20"/>
       <c r="J72" s="35"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73" s="20"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
+    <row r="73" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A73" s="28">
+        <v>12</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="20"/>
-      <c r="H73" s="20"/>
+      <c r="F73" s="21">
+        <v>44141</v>
+      </c>
+      <c r="G73" s="9">
+        <f ca="1">IF(H73="Done",0,(NETWORKDAYS.INTL(TODAY(),F73)))</f>
+        <v>39</v>
+      </c>
+      <c r="H73" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="I73" s="20"/>
       <c r="J73" s="35"/>
     </row>
@@ -3006,26 +3056,13 @@
       <c r="J75" s="35"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" s="20">
-        <v>13</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C76" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A76" s="20"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
       <c r="E76" s="21"/>
-      <c r="F76" s="21">
-        <v>44151</v>
-      </c>
-      <c r="G76" s="9">
-        <f ca="1">IF(H76="Done",0,(NETWORKDAYS.INTL(TODAY(),F76)))</f>
-        <v>45</v>
-      </c>
+      <c r="F76" s="21"/>
+      <c r="G76" s="20"/>
       <c r="H76" s="20"/>
       <c r="I76" s="20"/>
       <c r="J76" s="35"/>
@@ -3055,13 +3092,26 @@
       <c r="J78" s="35"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="20"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
+      <c r="A79" s="20">
+        <v>13</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="20"/>
+      <c r="F79" s="21">
+        <v>44151</v>
+      </c>
+      <c r="G79" s="9">
+        <f ca="1">IF(H79="Done",0,(NETWORKDAYS.INTL(TODAY(),F79)))</f>
+        <v>45</v>
+      </c>
       <c r="H79" s="20"/>
       <c r="I79" s="20"/>
       <c r="J79" s="35"/>
@@ -3090,27 +3140,14 @@
       <c r="I81" s="20"/>
       <c r="J81" s="35"/>
     </row>
-    <row r="82" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A82" s="20">
-        <v>14</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C82" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D82" s="20" t="s">
-        <v>25</v>
-      </c>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="20"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
       <c r="E82" s="21"/>
-      <c r="F82" s="21">
-        <v>44155</v>
-      </c>
-      <c r="G82" s="9">
-        <f ca="1">IF(H82="Done",0,(NETWORKDAYS.INTL(TODAY(),F82)))</f>
-        <v>49</v>
-      </c>
+      <c r="F82" s="21"/>
+      <c r="G82" s="20"/>
       <c r="H82" s="20"/>
       <c r="I82" s="20"/>
       <c r="J82" s="35"/>
@@ -3139,14 +3176,27 @@
       <c r="I84" s="20"/>
       <c r="J84" s="35"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" s="20"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="20"/>
+    <row r="85" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A85" s="20">
+        <v>14</v>
+      </c>
+      <c r="B85" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C85" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="20"/>
+      <c r="F85" s="21">
+        <v>44155</v>
+      </c>
+      <c r="G85" s="9">
+        <f ca="1">IF(H85="Done",0,(NETWORKDAYS.INTL(TODAY(),F85)))</f>
+        <v>49</v>
+      </c>
       <c r="H85" s="20"/>
       <c r="I85" s="20"/>
       <c r="J85" s="35"/>
@@ -3176,26 +3226,13 @@
       <c r="J87" s="35"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88" s="20">
-        <v>15</v>
-      </c>
-      <c r="B88" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C88" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D88" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A88" s="20"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="20"/>
       <c r="E88" s="21"/>
-      <c r="F88" s="21">
-        <v>44165</v>
-      </c>
-      <c r="G88" s="9">
-        <f t="shared" ref="G88" ca="1" si="0">(NETWORKDAYS.INTL(TODAY(),F88))</f>
-        <v>55</v>
-      </c>
+      <c r="F88" s="21"/>
+      <c r="G88" s="20"/>
       <c r="H88" s="20"/>
       <c r="I88" s="20"/>
       <c r="J88" s="35"/>
@@ -3225,13 +3262,26 @@
       <c r="J90" s="35"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A91" s="20"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="20"/>
-      <c r="D91" s="20"/>
+      <c r="A91" s="20">
+        <v>15</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="20"/>
+      <c r="F91" s="21">
+        <v>44165</v>
+      </c>
+      <c r="G91" s="9">
+        <f t="shared" ref="G91" ca="1" si="0">(NETWORKDAYS.INTL(TODAY(),F91))</f>
+        <v>55</v>
+      </c>
       <c r="H91" s="20"/>
       <c r="I91" s="20"/>
       <c r="J91" s="35"/>
@@ -3260,19 +3310,11 @@
       <c r="I93" s="20"/>
       <c r="J93" s="35"/>
     </row>
-    <row r="94" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="A94" s="20">
-        <v>16</v>
-      </c>
-      <c r="B94" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C94" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D94" s="20" t="s">
-        <v>25</v>
-      </c>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="20"/>
+      <c r="B94" s="17"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
       <c r="E94" s="21"/>
       <c r="F94" s="21"/>
       <c r="G94" s="20"/>
@@ -3304,11 +3346,19 @@
       <c r="I96" s="20"/>
       <c r="J96" s="35"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A97" s="20"/>
-      <c r="B97" s="17"/>
-      <c r="C97" s="20"/>
-      <c r="D97" s="20"/>
+    <row r="97" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A97" s="20">
+        <v>16</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C97" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E97" s="21"/>
       <c r="F97" s="21"/>
       <c r="G97" s="20"/>
@@ -3341,26 +3391,13 @@
       <c r="J99" s="35"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A100" s="20">
-        <v>17</v>
-      </c>
-      <c r="B100" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C100" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D100" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A100" s="20"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="20"/>
       <c r="E100" s="21"/>
-      <c r="F100" s="21">
-        <v>44172</v>
-      </c>
-      <c r="G100" s="9">
-        <f t="shared" ref="G100" ca="1" si="1">(NETWORKDAYS.INTL(TODAY(),F100))</f>
-        <v>60</v>
-      </c>
+      <c r="F100" s="21"/>
+      <c r="G100" s="20"/>
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
       <c r="J100" s="35"/>
@@ -3390,13 +3427,26 @@
       <c r="J102" s="35"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A103" s="20"/>
-      <c r="B103" s="17"/>
-      <c r="C103" s="20"/>
-      <c r="D103" s="20"/>
+      <c r="A103" s="20">
+        <v>17</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D103" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E103" s="21"/>
-      <c r="F103" s="21"/>
-      <c r="G103" s="20"/>
+      <c r="F103" s="21">
+        <v>44172</v>
+      </c>
+      <c r="G103" s="9">
+        <f t="shared" ref="G103" ca="1" si="1">(NETWORKDAYS.INTL(TODAY(),F103))</f>
+        <v>60</v>
+      </c>
       <c r="H103" s="20"/>
       <c r="I103" s="20"/>
       <c r="J103" s="35"/>
@@ -3438,26 +3488,13 @@
       <c r="J106" s="35"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A107" s="20">
-        <v>18</v>
-      </c>
-      <c r="B107" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C107" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D107" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="A107" s="20"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="20"/>
       <c r="E107" s="21"/>
-      <c r="F107" s="21">
-        <v>44176</v>
-      </c>
-      <c r="G107" s="9">
-        <f t="shared" ref="G107" ca="1" si="2">(NETWORKDAYS.INTL(TODAY(),F107))</f>
-        <v>64</v>
-      </c>
+      <c r="F107" s="21"/>
+      <c r="G107" s="20"/>
       <c r="H107" s="20"/>
       <c r="I107" s="20"/>
       <c r="J107" s="35"/>
@@ -3487,13 +3524,26 @@
       <c r="J109" s="35"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A110" s="20"/>
-      <c r="B110" s="17"/>
-      <c r="C110" s="20"/>
-      <c r="D110" s="20"/>
+      <c r="A110" s="20">
+        <v>18</v>
+      </c>
+      <c r="B110" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C110" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E110" s="21"/>
-      <c r="F110" s="21"/>
-      <c r="G110" s="20"/>
+      <c r="F110" s="21">
+        <v>44176</v>
+      </c>
+      <c r="G110" s="9">
+        <f t="shared" ref="G110" ca="1" si="2">(NETWORKDAYS.INTL(TODAY(),F110))</f>
+        <v>64</v>
+      </c>
       <c r="H110" s="20"/>
       <c r="I110" s="20"/>
       <c r="J110" s="35"/>
@@ -14023,37 +14073,40 @@
       <c r="J987" s="35"/>
     </row>
     <row r="988" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A988" s="22"/>
-      <c r="B988" s="12"/>
-      <c r="C988" s="22"/>
-      <c r="D988" s="22"/>
-      <c r="E988" s="23"/>
-      <c r="F988" s="23"/>
-      <c r="G988" s="22"/>
-      <c r="H988" s="22"/>
-      <c r="I988" s="22"/>
+      <c r="A988" s="20"/>
+      <c r="B988" s="17"/>
+      <c r="C988" s="20"/>
+      <c r="D988" s="20"/>
+      <c r="E988" s="21"/>
+      <c r="F988" s="21"/>
+      <c r="G988" s="20"/>
+      <c r="H988" s="20"/>
+      <c r="I988" s="20"/>
+      <c r="J988" s="35"/>
     </row>
     <row r="989" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A989" s="22"/>
-      <c r="B989" s="12"/>
-      <c r="C989" s="22"/>
-      <c r="D989" s="22"/>
-      <c r="E989" s="23"/>
-      <c r="F989" s="23"/>
-      <c r="G989" s="22"/>
-      <c r="H989" s="22"/>
-      <c r="I989" s="22"/>
+      <c r="A989" s="20"/>
+      <c r="B989" s="17"/>
+      <c r="C989" s="20"/>
+      <c r="D989" s="20"/>
+      <c r="E989" s="21"/>
+      <c r="F989" s="21"/>
+      <c r="G989" s="20"/>
+      <c r="H989" s="20"/>
+      <c r="I989" s="20"/>
+      <c r="J989" s="35"/>
     </row>
     <row r="990" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A990" s="22"/>
-      <c r="B990" s="12"/>
-      <c r="C990" s="22"/>
-      <c r="D990" s="22"/>
-      <c r="E990" s="23"/>
-      <c r="F990" s="23"/>
-      <c r="G990" s="22"/>
-      <c r="H990" s="22"/>
-      <c r="I990" s="22"/>
+      <c r="A990" s="20"/>
+      <c r="B990" s="17"/>
+      <c r="C990" s="20"/>
+      <c r="D990" s="20"/>
+      <c r="E990" s="21"/>
+      <c r="F990" s="21"/>
+      <c r="G990" s="20"/>
+      <c r="H990" s="20"/>
+      <c r="I990" s="20"/>
+      <c r="J990" s="35"/>
     </row>
     <row r="991" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A991" s="22"/>
@@ -14110,6 +14163,39 @@
       <c r="H995" s="22"/>
       <c r="I995" s="22"/>
     </row>
+    <row r="996" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A996" s="22"/>
+      <c r="B996" s="12"/>
+      <c r="C996" s="22"/>
+      <c r="D996" s="22"/>
+      <c r="E996" s="23"/>
+      <c r="F996" s="23"/>
+      <c r="G996" s="22"/>
+      <c r="H996" s="22"/>
+      <c r="I996" s="22"/>
+    </row>
+    <row r="997" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A997" s="22"/>
+      <c r="B997" s="12"/>
+      <c r="C997" s="22"/>
+      <c r="D997" s="22"/>
+      <c r="E997" s="23"/>
+      <c r="F997" s="23"/>
+      <c r="G997" s="22"/>
+      <c r="H997" s="22"/>
+      <c r="I997" s="22"/>
+    </row>
+    <row r="998" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A998" s="22"/>
+      <c r="B998" s="12"/>
+      <c r="C998" s="22"/>
+      <c r="D998" s="22"/>
+      <c r="E998" s="23"/>
+      <c r="F998" s="23"/>
+      <c r="G998" s="22"/>
+      <c r="H998" s="22"/>
+      <c r="I998" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:G3"/>
@@ -14117,52 +14203,52 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="H3:J3"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="75" priority="63" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="74" priority="66" stopIfTrue="1" operator="equal">
       <formula>"DELAY"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="73" priority="62" stopIfTrue="1" operator="equal">
       <formula>"DELAY"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="72" priority="59" stopIfTrue="1" operator="equal">
       <formula>"DELAY"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="71" priority="61" stopIfTrue="1" operator="equal">
       <formula>"DONE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="70" priority="64" stopIfTrue="1" operator="equal">
       <formula>"O"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="69" priority="60" stopIfTrue="1" operator="equal">
       <formula>"ONGOING"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="68" priority="67" stopIfTrue="1" operator="equal">
       <formula>"ONGOING"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="67" priority="65" stopIfTrue="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I21">
+  <conditionalFormatting sqref="H5:I24">
     <cfRule type="cellIs" dxfId="66" priority="68" stopIfTrue="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
@@ -14367,20 +14453,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
       <c r="L1" s="2" t="s">
         <v>10</v>
@@ -14396,18 +14482,18 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="45" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
       <c r="M2" s="3" t="s">
         <v>32</v>
@@ -14417,18 +14503,18 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="45" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
       <c r="M3" s="3" t="s">
         <v>16</v>
@@ -14812,7 +14898,7 @@
       <c r="K19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="11" t="s">
         <v>79</v>
@@ -14831,7 +14917,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -14845,7 +14931,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="24">
         <v>3</v>
       </c>
@@ -14873,7 +14959,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15" t="s">
         <v>81</v>
@@ -14899,7 +14985,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" ht="42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="13" t="s">
         <v>82</v>
@@ -14925,7 +15011,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
Added questions and modified draft concept
</commit_message>
<xml_diff>
--- a/ECE 4981 Task List.xlsx
+++ b/ECE 4981 Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fall2020\ECE4981\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70950ECB-3449-458E-A06B-A18C6B50627D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F523B0-585C-4DAE-8A2E-5FCB7E2B26FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8829020-0EF2-4875-8210-9C2942B344E7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="97">
   <si>
     <t>START DATE</t>
   </si>
@@ -1700,8 +1700,8 @@
   <dimension ref="A1:P998"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+      <pane ySplit="4" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="G14" s="9">
         <f ca="1">IF(H14="Done",0,(NETWORKDAYS.INTL(TODAY(),F14)))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>17</v>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I16" s="43"/>
       <c r="J16" s="34" t="s">
@@ -2124,7 +2124,9 @@
       <c r="B17" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="14"/>
+      <c r="C17" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="D17" s="6" t="s">
         <v>25</v>
       </c>
@@ -2147,7 +2149,9 @@
       <c r="B18" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="D18" s="6" t="s">
         <v>25</v>
       </c>
@@ -2180,7 +2184,7 @@
       </c>
       <c r="G19" s="9">
         <f ca="1">IF(H19="Done",0,(NETWORKDAYS.INTL(TODAY(),F19)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>32</v>
@@ -2206,7 +2210,7 @@
       </c>
       <c r="G20" s="9">
         <f ca="1">IF(H20="Done",0,(NETWORKDAYS.INTL(TODAY(),F20)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>32</v>
@@ -2232,7 +2236,7 @@
       </c>
       <c r="G21" s="9">
         <f ca="1">IF(H21="Done",0,(NETWORKDAYS.INTL(TODAY(),F21)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>32</v>
@@ -2277,7 +2281,7 @@
       </c>
       <c r="G23" s="9">
         <f ca="1">IF(H23="Done",0,(NETWORKDAYS.INTL(TODAY(),F23)))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>32</v>
@@ -2367,7 +2371,7 @@
       </c>
       <c r="G28" s="9">
         <f ca="1">IF(H28="Done",0,(NETWORKDAYS.INTL(TODAY(),F28)))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28" s="20" t="s">
         <v>32</v>
@@ -2481,7 +2485,7 @@
       </c>
       <c r="G35" s="9">
         <f ca="1">IF(H35="Done",0,(NETWORKDAYS.INTL(TODAY(),F35)))</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H35" s="20" t="s">
         <v>32</v>
@@ -2580,7 +2584,7 @@
       </c>
       <c r="G42" s="9">
         <f ca="1">IF(H42="Done",0,(NETWORKDAYS.INTL(TODAY(),F42)))</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
@@ -2677,7 +2681,7 @@
       </c>
       <c r="G49" s="9">
         <f ca="1">IF(H49="Done",0,(NETWORKDAYS.INTL(TODAY(),F49)))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H49" s="20" t="s">
         <v>32</v>
@@ -2764,7 +2768,7 @@
       </c>
       <c r="G55" s="9">
         <f ca="1">IF(H55="Done",0,(NETWORKDAYS.INTL(TODAY(),F55)))</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H55" s="20" t="s">
         <v>32</v>
@@ -2851,7 +2855,7 @@
       </c>
       <c r="G61" s="9">
         <f ca="1">IF(H61="Done",0,(NETWORKDAYS.INTL(TODAY(),F61)))</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H61" s="20" t="s">
         <v>32</v>
@@ -2938,7 +2942,7 @@
       </c>
       <c r="G67" s="9">
         <f ca="1">IF(H67="Done",0,(NETWORKDAYS.INTL(TODAY(),F67)))</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H67" s="20" t="s">
         <v>32</v>
@@ -3025,7 +3029,7 @@
       </c>
       <c r="G73" s="9">
         <f ca="1">IF(H73="Done",0,(NETWORKDAYS.INTL(TODAY(),F73)))</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H73" s="20" t="s">
         <v>32</v>
@@ -3112,7 +3116,7 @@
       </c>
       <c r="G79" s="9">
         <f ca="1">IF(H79="Done",0,(NETWORKDAYS.INTL(TODAY(),F79)))</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H79" s="20"/>
       <c r="I79" s="20"/>
@@ -3197,7 +3201,7 @@
       </c>
       <c r="G85" s="9">
         <f ca="1">IF(H85="Done",0,(NETWORKDAYS.INTL(TODAY(),F85)))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H85" s="20"/>
       <c r="I85" s="20"/>
@@ -3282,7 +3286,7 @@
       </c>
       <c r="G91" s="9">
         <f t="shared" ref="G91" ca="1" si="0">(NETWORKDAYS.INTL(TODAY(),F91))</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H91" s="20"/>
       <c r="I91" s="20"/>
@@ -3447,7 +3451,7 @@
       </c>
       <c r="G103" s="9">
         <f t="shared" ref="G103" ca="1" si="1">(NETWORKDAYS.INTL(TODAY(),F103))</f>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H103" s="20"/>
       <c r="I103" s="20"/>
@@ -3544,7 +3548,7 @@
       </c>
       <c r="G110" s="9">
         <f t="shared" ref="G110" ca="1" si="2">(NETWORKDAYS.INTL(TODAY(),F110))</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H110" s="20"/>
       <c r="I110" s="20"/>
@@ -14580,7 +14584,7 @@
       </c>
       <c r="G5" s="42">
         <f t="shared" ref="G5" ca="1" si="0">(NETWORKDAYS.INTL(TODAY(),F5))</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -14605,7 +14609,7 @@
       </c>
       <c r="G6" s="9">
         <f ca="1">IF(H6="Done",0,(NETWORKDAYS.INTL(TODAY(),F6)))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -14629,7 +14633,7 @@
       </c>
       <c r="G7" s="9">
         <f ca="1">IF(H7="Done",0,(NETWORKDAYS.INTL(TODAY(),F7)))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -14653,7 +14657,7 @@
       </c>
       <c r="G8" s="9">
         <f ca="1">IF(H8="Done",0,(NETWORKDAYS.INTL(TODAY(),F8)))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -14677,7 +14681,7 @@
       </c>
       <c r="G9" s="9">
         <f ca="1">IF(H9="Done",0,(NETWORKDAYS.INTL(TODAY(),F9)))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -14718,7 +14722,7 @@
       </c>
       <c r="G11" s="9">
         <f ca="1">IF(H11="Done",0,(NETWORKDAYS.INTL(TODAY(),F11)))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -14742,7 +14746,7 @@
       </c>
       <c r="G12" s="9">
         <f ca="1">IF(H12="Done",0,(NETWORKDAYS.INTL(TODAY(),F12)))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -14781,7 +14785,7 @@
       </c>
       <c r="G14" s="42">
         <f t="shared" ref="G14" ca="1" si="1">(NETWORKDAYS.INTL(TODAY(),F14))</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -14806,7 +14810,7 @@
       </c>
       <c r="G15" s="9">
         <f ca="1">IF(H15="Done",0,(NETWORKDAYS.INTL(TODAY(),F15)))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -14831,7 +14835,7 @@
       </c>
       <c r="G16" s="9">
         <f ca="1">IF(H16="Done",0,(NETWORKDAYS.INTL(TODAY(),F16)))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -14856,7 +14860,7 @@
       </c>
       <c r="G17" s="9">
         <f ca="1">IF(H17="Done",0,(NETWORKDAYS.INTL(TODAY(),F17)))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -14952,7 +14956,7 @@
       </c>
       <c r="G22" s="42">
         <f t="shared" ref="G22" ca="1" si="2">(NETWORKDAYS.INTL(TODAY(),F22))</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -14978,7 +14982,7 @@
       </c>
       <c r="G23" s="9">
         <f ca="1">IF(H23="Done",0,(NETWORKDAYS.INTL(TODAY(),F23)))</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -15004,7 +15008,7 @@
       </c>
       <c r="G24" s="9">
         <f ca="1">IF(H24="Done",0,(NETWORKDAYS.INTL(TODAY(),F24)))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -15030,7 +15034,7 @@
       </c>
       <c r="G25" s="9">
         <f ca="1">IF(H25="Done",0,(NETWORKDAYS.INTL(TODAY(),F25)))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -15056,7 +15060,7 @@
       </c>
       <c r="G26" s="9">
         <f ca="1">IF(H26="Done",0,(NETWORKDAYS.INTL(TODAY(),F26)))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -15082,7 +15086,7 @@
       </c>
       <c r="G27" s="9">
         <f ca="1">IF(H27="Done",0,(NETWORKDAYS.INTL(TODAY(),F27)))</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>

</xml_diff>